<commit_message>
ranges around GC min table
</commit_message>
<xml_diff>
--- a/dist_min_to_oriC.xlsx
+++ b/dist_min_to_oriC.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lena\seqinf_detection_replication_origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23888F28-61F5-45D8-884E-8CC1F3A02D1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8361316-B062-45CD-AD6A-22487D828E9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5568" yWindow="228" windowWidth="11352" windowHeight="11688" activeTab="1"/>
+    <workbookView xWindow="5568" yWindow="228" windowWidth="11352" windowHeight="11688" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E.coli" sheetId="1" r:id="rId1"/>
     <sheet name="Vibrio" sheetId="2" r:id="rId2"/>
+    <sheet name="S.enterica" sheetId="3" r:id="rId3"/>
+    <sheet name="Thermotoga" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>Strain</t>
   </si>
@@ -190,13 +192,143 @@
   </si>
   <si>
     <t>Vibrio cholerae strain NCTC9420 chromosome 1, complete sequence</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Typhi str. CT18</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Paratyphi A str. ATCC 9150</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Paratyphi B str. SPB7</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Enteritidis str. P125109</t>
+  </si>
+  <si>
+    <t>Salmonella enterica strain FORC_038, 
+complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Enteritidis str. EC20120008, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Agona str. 460004 2-1, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+strain YU39, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Thompson strain RM1986, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica strain LT2, 
+complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Infantis strain FSIS1502916, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Heidelberg strain SA02DT09004001 chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Enteritidis strain FORC_052 chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Senftenberg strain 775W chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Saintpaul str. SARA26 chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Nitra strain S-1687 chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica strain RM11065 
+chromosome, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Abaetetuba str. ATCC 35640, complete genome</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica 
+serovar Anatum str. ATCC BAA-1592, complete genome</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>Thermotoga petrophila RKU-1</t>
+  </si>
+  <si>
+    <t>Thermotoga maritima MSB8</t>
+  </si>
+  <si>
+    <t>Thermotoga lettingae TMO</t>
+  </si>
+  <si>
+    <t>Thermotoga sp. RQ2</t>
+  </si>
+  <si>
+    <t>Thermotoga neapolitana DSM 4359</t>
+  </si>
+  <si>
+    <t>Thermotoga naphthophila RKU-10</t>
+  </si>
+  <si>
+    <t>Thermotoga thermarum DSM 5069 
+chromosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermotoga caldifontis AZM44c09 DNA </t>
+  </si>
+  <si>
+    <t>Thermotoga sp. 2812B</t>
+  </si>
+  <si>
+    <t>Thermotoga sp. Cell2</t>
+  </si>
+  <si>
+    <t>Pseudothermotoga hypogea DSM 
+11164 = NBRC 106472 chromosome</t>
+  </si>
+  <si>
+    <t>Thermotoga sp. RQ7</t>
+  </si>
+  <si>
+    <t>Thermotoga maritima strain Tma200</t>
+  </si>
+  <si>
+    <t>Thermotoga maritima strain Tma100</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>Max range 
+around minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,16 +357,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -242,11 +394,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -280,12 +460,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -593,11 +800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:F49"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +831,9 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -648,6 +857,10 @@
         <f t="shared" ref="F2:F20" si="1">D2-B2</f>
         <v>414</v>
       </c>
+      <c r="G2">
+        <f>ABS(E2)+ABS(F2)</f>
+        <v>451</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -670,6 +883,10 @@
         <f t="shared" si="1"/>
         <v>4703492</v>
       </c>
+      <c r="G3" s="18">
+        <f t="shared" ref="G3:G20" si="2">ABS(E3)+ABS(F3)</f>
+        <v>9406607</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -692,6 +909,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -714,6 +935,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -736,6 +961,10 @@
         <f t="shared" si="1"/>
         <v>4587988</v>
       </c>
+      <c r="G6" s="18">
+        <f t="shared" si="2"/>
+        <v>9175599</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -758,6 +987,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G7" s="22">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -780,6 +1013,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -802,6 +1039,10 @@
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -824,6 +1065,10 @@
         <f t="shared" si="1"/>
         <v>4868948</v>
       </c>
+      <c r="G10" s="18">
+        <f t="shared" si="2"/>
+        <v>9737519</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -846,6 +1091,10 @@
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -868,6 +1117,10 @@
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -890,6 +1143,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -912,6 +1169,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -934,6 +1195,10 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -956,8 +1221,12 @@
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -978,8 +1247,12 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1000,8 +1273,12 @@
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1022,8 +1299,12 @@
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1043,6 +1324,22 @@
       <c r="F20">
         <f t="shared" si="1"/>
         <v>414</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="20">
+        <f>MAX(G11,G12,G13,G14,G15,G16:G20,G2,G4,G5,G7,G8,G9)</f>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -1052,11 +1349,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1361,7 @@
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1083,8 +1380,11 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -1105,8 +1405,12 @@
         <f t="shared" ref="F2:F20" si="1">D2-B2</f>
         <v>-3919892</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G2" s="18">
+        <f>ABS(E2)+ABS(F2)</f>
+        <v>3928047</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
@@ -1127,8 +1431,12 @@
         <f t="shared" si="1"/>
         <v>-4042362</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G3" s="18">
+        <f t="shared" ref="G3:G20" si="2">ABS(E3)+ABS(F3)</f>
+        <v>4077152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1149,8 +1457,12 @@
         <f t="shared" si="1"/>
         <v>-8153</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>16616</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
@@ -1171,8 +1483,12 @@
         <f t="shared" si="1"/>
         <v>-8464</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>18331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -1193,8 +1509,12 @@
         <f t="shared" si="1"/>
         <v>7410</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>14510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1215,8 +1535,12 @@
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="18">
+        <f t="shared" si="2"/>
+        <v>2961279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>31</v>
       </c>
@@ -1237,8 +1561,12 @@
         <f t="shared" si="1"/>
         <v>-1423</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>11290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>32</v>
       </c>
@@ -1259,8 +1587,12 @@
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G9" s="18">
+        <f t="shared" si="2"/>
+        <v>2892653</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
@@ -1281,8 +1613,12 @@
         <f t="shared" si="1"/>
         <v>8471</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>16632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
@@ -1303,8 +1639,12 @@
         <f t="shared" si="1"/>
         <v>7410</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>14510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
@@ -1325,8 +1665,12 @@
         <f t="shared" si="1"/>
         <v>1752</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
@@ -1347,8 +1691,12 @@
         <f t="shared" si="1"/>
         <v>-1286</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>11153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
@@ -1369,8 +1717,12 @@
         <f t="shared" si="1"/>
         <v>-2936683</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G14" s="18">
+        <f t="shared" si="2"/>
+        <v>2936705</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1391,8 +1743,12 @@
         <f t="shared" si="1"/>
         <v>-3032889</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G15" s="18">
+        <f t="shared" si="2"/>
+        <v>6066088</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1413,8 +1769,12 @@
         <f t="shared" si="1"/>
         <v>-255</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1795,12 @@
         <f t="shared" si="1"/>
         <v>1054</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G17" s="18">
+        <f t="shared" si="2"/>
+        <v>1073011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,8 +1821,12 @@
         <f t="shared" si="1"/>
         <v>8471</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>16632</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
@@ -1479,8 +1847,12 @@
         <f t="shared" si="1"/>
         <v>7410</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>14510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -1500,6 +1872,1027 @@
       <c r="F20" s="11">
         <f t="shared" si="1"/>
         <v>7410</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>14510</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="20">
+        <f>MAX(G20,G19,G18,G16,G13,G12,G11,G10,G6,G5,G4)</f>
+        <v>18331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2592DB1-5D52-4B0A-98C1-B894DC066C86}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>3764856</v>
+      </c>
+      <c r="C2">
+        <v>3765058</v>
+      </c>
+      <c r="D2">
+        <v>3765435</v>
+      </c>
+      <c r="E2" s="14">
+        <f>C2-B2</f>
+        <v>202</v>
+      </c>
+      <c r="F2" s="14">
+        <f>D2-B2</f>
+        <v>579</v>
+      </c>
+      <c r="G2">
+        <f>ABS(E2)+ABS(F2)</f>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>3859383</v>
+      </c>
+      <c r="C3">
+        <v>3858807</v>
+      </c>
+      <c r="D3">
+        <v>3859184</v>
+      </c>
+      <c r="E3" s="14">
+        <f t="shared" ref="E3:E20" si="0">C3-B3</f>
+        <v>-576</v>
+      </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="F3:F20" si="1">D3-B3</f>
+        <v>-199</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G20" si="2">ABS(E3)+ABS(F3)</f>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>4028937</v>
+      </c>
+      <c r="C4">
+        <v>4028361</v>
+      </c>
+      <c r="D4">
+        <v>4028738</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>3954702</v>
+      </c>
+      <c r="C5">
+        <v>3954126</v>
+      </c>
+      <c r="D5">
+        <v>3954503</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>4902632</v>
+      </c>
+      <c r="C6">
+        <v>1268199</v>
+      </c>
+      <c r="D6">
+        <v>1269338</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="0"/>
+        <v>-3634433</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="1"/>
+        <v>-3633294</v>
+      </c>
+      <c r="G6" s="18">
+        <f t="shared" si="2"/>
+        <v>7267727</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>3977342</v>
+      </c>
+      <c r="C7">
+        <v>3976766</v>
+      </c>
+      <c r="D7">
+        <v>3977143</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>1035446</v>
+      </c>
+      <c r="C8">
+        <v>1034870</v>
+      </c>
+      <c r="D8">
+        <v>1035247</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>4112370</v>
+      </c>
+      <c r="C9">
+        <v>4111794</v>
+      </c>
+      <c r="D9">
+        <v>4112171</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>3931243</v>
+      </c>
+      <c r="C10">
+        <v>3930667</v>
+      </c>
+      <c r="D10">
+        <v>3931044</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>1572949</v>
+      </c>
+      <c r="C11">
+        <v>1573151</v>
+      </c>
+      <c r="D11">
+        <v>1573528</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="0"/>
+        <v>202</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
+        <v>579</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12">
+        <v>4499368</v>
+      </c>
+      <c r="C12">
+        <v>4498792</v>
+      </c>
+      <c r="D12">
+        <v>4499169</v>
+      </c>
+      <c r="E12" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <v>4012390</v>
+      </c>
+      <c r="C13">
+        <v>4011814</v>
+      </c>
+      <c r="D13">
+        <v>4012191</v>
+      </c>
+      <c r="E13" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>697</v>
+      </c>
+      <c r="C14">
+        <v>4651363</v>
+      </c>
+      <c r="D14">
+        <v>4651740</v>
+      </c>
+      <c r="E14" s="14">
+        <f t="shared" si="0"/>
+        <v>4650666</v>
+      </c>
+      <c r="F14" s="14">
+        <f t="shared" si="1"/>
+        <v>4651043</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="2"/>
+        <v>9301709</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>4920459</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>378</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="0"/>
+        <v>-4920458</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="1"/>
+        <v>-4920081</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="2"/>
+        <v>9840539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16">
+        <v>766</v>
+      </c>
+      <c r="C16">
+        <v>4646673</v>
+      </c>
+      <c r="D16">
+        <v>4647050</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" si="0"/>
+        <v>4645907</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="1"/>
+        <v>4646284</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="2"/>
+        <v>9292191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>3960409</v>
+      </c>
+      <c r="C17">
+        <v>3959833</v>
+      </c>
+      <c r="D17">
+        <v>3960210</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <v>4233587</v>
+      </c>
+      <c r="C18">
+        <v>4233011</v>
+      </c>
+      <c r="D18">
+        <v>4233388</v>
+      </c>
+      <c r="E18" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F18" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>1145764</v>
+      </c>
+      <c r="C19">
+        <v>1145188</v>
+      </c>
+      <c r="D19">
+        <v>1145565</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" si="0"/>
+        <v>-576</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="1"/>
+        <v>-199</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>3110111</v>
+      </c>
+      <c r="C20">
+        <v>3110313</v>
+      </c>
+      <c r="D20">
+        <v>3110690</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="0"/>
+        <v>202</v>
+      </c>
+      <c r="F20" s="14">
+        <f t="shared" si="1"/>
+        <v>579</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="G22" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="16"/>
+      <c r="G23" s="20">
+        <f>MAX(G20,G19,G18,G17,G13,G12,G11,G10,G9,G8,G7,G5,G4,G3,G2)</f>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814FC12-D546-4198-B997-6A1CF2F1B7E6}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>787199</v>
+      </c>
+      <c r="C2">
+        <v>786686</v>
+      </c>
+      <c r="D2">
+        <v>787242</v>
+      </c>
+      <c r="E2">
+        <f>C2-B2</f>
+        <v>-513</v>
+      </c>
+      <c r="F2">
+        <f>D2-B2</f>
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <f>ABS(E2)+ABS(F2)</f>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>156978</v>
+      </c>
+      <c r="C3">
+        <v>156961</v>
+      </c>
+      <c r="D3">
+        <v>157517</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E20" si="0">C3-B3</f>
+        <v>-17</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F20" si="1">D3-B3</f>
+        <v>539</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G16" si="2">ABS(E3)+ABS(F3)</f>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>140889</v>
+      </c>
+      <c r="C4">
+        <v>157248</v>
+      </c>
+      <c r="D4">
+        <v>157755</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>16359</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>16866</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="2"/>
+        <v>33225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>822207</v>
+      </c>
+      <c r="C5">
+        <v>821694</v>
+      </c>
+      <c r="D5">
+        <v>822250</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>-513</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>539312</v>
+      </c>
+      <c r="C6">
+        <v>539224</v>
+      </c>
+      <c r="D6">
+        <v>539439</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>-88</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>141850</v>
+      </c>
+      <c r="C7">
+        <v>807603</v>
+      </c>
+      <c r="D7">
+        <v>808159</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>665753</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>666309</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" si="2"/>
+        <v>1332062</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8">
+        <v>12255</v>
+      </c>
+      <c r="C8">
+        <v>2026649</v>
+      </c>
+      <c r="D8">
+        <v>2028223</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2014394</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2015968</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="2"/>
+        <v>4030362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>788618</v>
+      </c>
+      <c r="C9">
+        <v>788099</v>
+      </c>
+      <c r="D9">
+        <v>788661</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-519</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10">
+        <v>210774</v>
+      </c>
+      <c r="C10">
+        <v>315913</v>
+      </c>
+      <c r="D10">
+        <v>316450</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>105139</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>105676</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="2"/>
+        <v>210815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11">
+        <v>826973</v>
+      </c>
+      <c r="C11">
+        <v>826460</v>
+      </c>
+      <c r="D11">
+        <v>827016</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-513</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>772324</v>
+      </c>
+      <c r="C12">
+        <v>771811</v>
+      </c>
+      <c r="D12">
+        <v>772367</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-513</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>1198932</v>
+      </c>
+      <c r="C13">
+        <v>1124232</v>
+      </c>
+      <c r="D13">
+        <v>1124765</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-74700</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>-74167</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="2"/>
+        <v>148867</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>816438</v>
+      </c>
+      <c r="C14">
+        <v>816027</v>
+      </c>
+      <c r="D14">
+        <v>816571</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>-411</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15">
+        <v>156978</v>
+      </c>
+      <c r="C15">
+        <v>156961</v>
+      </c>
+      <c r="D15">
+        <v>157517</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-17</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>539</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16">
+        <v>156978</v>
+      </c>
+      <c r="C16">
+        <v>156961</v>
+      </c>
+      <c r="D16">
+        <v>157517</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>-17</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>539</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="21">
+        <f>MAX(G2,G3,G5,G6,G9,G11,G12,G15,G14,G16)</f>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>